<commit_message>
Alle Diagramme erstellt und formatiert
</commit_message>
<xml_diff>
--- a/documents/marketing/Umfrage-I Ergebnisse 21.12.2014.xlsx
+++ b/documents/marketing/Umfrage-I Ergebnisse 21.12.2014.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="315" windowWidth="23475" windowHeight="9765" tabRatio="728" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="315" windowWidth="23475" windowHeight="9765" tabRatio="728" firstSheet="1" activeTab="25"/>
   </bookViews>
   <sheets>
     <sheet name="Alle Ergebnisse" sheetId="1" r:id="rId1"/>
@@ -1726,8 +1726,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="23" x14ac:knownFonts="1">
     <font>
@@ -2293,11 +2294,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2345,6 +2346,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF5722"/>
+      <color rgb="FF00C853"/>
+      <color rgb="FF3F51B5"/>
+      <color rgb="FFF50057"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2370,8 +2379,10 @@
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
-      <c:pieChart>
-        <c:varyColors val="1"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="0"/>
@@ -2386,6 +2397,12 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF5722"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLbl>
               <c:idx val="4"/>
@@ -2408,7 +2425,7 @@
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="1"/>
+            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -2465,16 +2482,43 @@
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="1"/>
         </c:dLbls>
-        <c:firstSliceAng val="0"/>
-      </c:pieChart>
+        <c:gapWidth val="100"/>
+        <c:axId val="153503232"/>
+        <c:axId val="153504768"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="153503232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="153504768"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="153504768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="153503232"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -2522,6 +2566,11 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF5722"/>
+            </a:solidFill>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -2611,7 +2660,7 @@
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2620,10 +2669,6 @@
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -2653,8 +2698,10 @@
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
-      <c:pieChart>
-        <c:varyColors val="1"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="0"/>
@@ -2669,6 +2716,12 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF5722"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
@@ -2676,7 +2729,7 @@
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="1"/>
+            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -2727,25 +2780,43 @@
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="1"/>
         </c:dLbls>
-        <c:firstSliceAng val="0"/>
-      </c:pieChart>
+        <c:gapWidth val="100"/>
+        <c:axId val="190228352"/>
+        <c:axId val="190229504"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="190228352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="190229504"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="190229504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="190228352"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr rtl="0">
-            <a:defRPr/>
-          </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -2791,10 +2862,42 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="3F51B5"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00C853"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF5722"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="F50057"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
           <c:dLbls>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
-            <c:showCatName val="0"/>
+            <c:showCatName val="1"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
@@ -2848,10 +2951,6 @@
         <c:firstSliceAng val="0"/>
       </c:pieChart>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -2897,10 +2996,24 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF5722"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00C853"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
           <c:dLbls>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
-            <c:showCatName val="0"/>
+            <c:showCatName val="1"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
@@ -2948,10 +3061,6 @@
         <c:firstSliceAng val="0"/>
       </c:pieChart>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -2997,10 +3106,24 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="00C853"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF5722"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
           <c:dLbls>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
-            <c:showCatName val="0"/>
+            <c:showCatName val="1"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
@@ -3048,10 +3171,6 @@
         <c:firstSliceAng val="0"/>
       </c:pieChart>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -3099,6 +3218,11 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF5722"/>
+            </a:solidFill>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -3184,7 +3308,7 @@
       <c:catAx>
         <c:axId val="143946112"/>
         <c:scaling>
-          <c:orientation val="minMax"/>
+          <c:orientation val="maxMin"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3204,9 +3328,9 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
+        <c:axPos val="t"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3215,10 +3339,6 @@
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -3266,6 +3386,11 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF5722"/>
+            </a:solidFill>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -3363,7 +3488,7 @@
       <c:catAx>
         <c:axId val="144030336"/>
         <c:scaling>
-          <c:orientation val="minMax"/>
+          <c:orientation val="maxMin"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3383,9 +3508,9 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
+        <c:axPos val="t"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3394,10 +3519,6 @@
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -3444,6 +3565,51 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:marker>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF5722"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="3F51B5"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="FF5722"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="FF5722"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="FF5722"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
           <c:dLbls>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
@@ -3519,6 +3685,16 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="-5400000" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="144247040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
@@ -3543,10 +3719,6 @@
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -3592,10 +3764,28 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00C853"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF5722"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
           <c:dLbls>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
-            <c:showCatName val="0"/>
+            <c:showCatName val="1"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
@@ -3643,10 +3833,6 @@
         <c:firstSliceAng val="0"/>
       </c:pieChart>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -3676,8 +3862,10 @@
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
-      <c:pieChart>
-        <c:varyColors val="1"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="0"/>
@@ -3692,6 +3880,12 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF5722"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
@@ -3699,7 +3893,7 @@
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="1"/>
+            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -3750,15 +3944,43 @@
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="1"/>
         </c:dLbls>
-        <c:firstSliceAng val="0"/>
-      </c:pieChart>
+        <c:gapWidth val="100"/>
+        <c:axId val="16935936"/>
+        <c:axId val="156020736"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="16935936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="156020736"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="156020736"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="16935936"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -3806,6 +4028,11 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF5722"/>
+            </a:solidFill>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -3891,7 +4118,7 @@
       <c:catAx>
         <c:axId val="182309632"/>
         <c:scaling>
-          <c:orientation val="minMax"/>
+          <c:orientation val="maxMin"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3911,9 +4138,9 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
+        <c:axPos val="t"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3922,10 +4149,6 @@
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -3955,8 +4178,10 @@
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
-      <c:pieChart>
-        <c:varyColors val="1"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="0"/>
@@ -3971,6 +4196,12 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF5722"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
@@ -3978,7 +4209,7 @@
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="1"/>
+            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -4029,15 +4260,43 @@
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="1"/>
         </c:dLbls>
-        <c:firstSliceAng val="0"/>
-      </c:pieChart>
+        <c:gapWidth val="100"/>
+        <c:axId val="156318720"/>
+        <c:axId val="183636736"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="156318720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="183636736"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="183636736"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="156318720"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -4067,8 +4326,10 @@
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
-      <c:pieChart>
-        <c:varyColors val="1"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="0"/>
@@ -4083,6 +4344,12 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF5722"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
@@ -4090,7 +4357,7 @@
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="1"/>
+            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -4153,16 +4420,43 @@
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="1"/>
         </c:dLbls>
-        <c:firstSliceAng val="0"/>
-      </c:pieChart>
+        <c:gapWidth val="100"/>
+        <c:axId val="192124800"/>
+        <c:axId val="192126336"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="192124800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="192126336"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="192126336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="192124800"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -4210,6 +4504,11 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF5722"/>
+            </a:solidFill>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -4289,7 +4588,7 @@
       <c:catAx>
         <c:axId val="182626944"/>
         <c:scaling>
-          <c:orientation val="minMax"/>
+          <c:orientation val="maxMin"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -4310,9 +4609,9 @@
           <c:max val="1"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
+        <c:axPos val="t"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4321,10 +4620,6 @@
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -4354,8 +4649,10 @@
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
-      <c:pieChart>
-        <c:varyColors val="1"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="0"/>
@@ -4370,6 +4667,12 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF5722"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
@@ -4377,7 +4680,7 @@
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="1"/>
+            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -4428,15 +4731,44 @@
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="1"/>
         </c:dLbls>
-        <c:firstSliceAng val="0"/>
-      </c:pieChart>
+        <c:gapWidth val="100"/>
+        <c:axId val="184931840"/>
+        <c:axId val="184933376"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="184931840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="184933376"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="184933376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.70000000000000007"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="184931840"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -4466,8 +4798,10 @@
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
-      <c:pieChart>
-        <c:varyColors val="1"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="0"/>
@@ -4482,6 +4816,12 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF5722"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
@@ -4489,7 +4829,7 @@
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="1"/>
+            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -4546,25 +4886,44 @@
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="1"/>
         </c:dLbls>
-        <c:firstSliceAng val="0"/>
-      </c:pieChart>
+        <c:gapWidth val="100"/>
+        <c:axId val="132610688"/>
+        <c:axId val="187832192"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="132610688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="187832192"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="187832192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="132610688"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr rtl="0">
-            <a:defRPr/>
-          </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -4612,6 +4971,11 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF5722"/>
+            </a:solidFill>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -4697,7 +5061,7 @@
       <c:catAx>
         <c:axId val="182785920"/>
         <c:scaling>
-          <c:orientation val="minMax"/>
+          <c:orientation val="maxMin"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -4717,9 +5081,9 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
+        <c:axPos val="t"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4728,10 +5092,6 @@
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -4777,10 +5137,28 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00C853"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF5722"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
           <c:dLbls>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
-            <c:showCatName val="0"/>
+            <c:showCatName val="1"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
@@ -4828,10 +5206,6 @@
         <c:firstSliceAng val="0"/>
       </c:pieChart>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -4866,154 +5240,165 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="2"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Q8'!$A$2</c:f>
+              <c:f>'Q8'!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>N</c:v>
+                  <c:v>% der Fälle</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF5722"/>
+            </a:solidFill>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'Q8'!$B$1:$U$1</c:f>
+              <c:f>'Q8'!$B$1:$V$1</c:f>
               <c:numCache>
-                <c:formatCode>0</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>50</c:v>
-                </c:pt>
                 <c:pt idx="11">
-                  <c:v>55</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>60</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>65</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>70</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>75</c:v>
+                  <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>80</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>85</c:v>
+                  <c:v>8.5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>90</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>95</c:v>
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Q8'!$B$2:$U$2</c:f>
+              <c:f>'Q8'!$B$4:$V$4</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>3.125E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>1.0416666666666666E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>3.125E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9</c:v>
+                  <c:v>4.6875E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>2.6041666666666668E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12</c:v>
+                  <c:v>6.25E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11</c:v>
+                  <c:v>5.7291666666666664E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4</c:v>
+                  <c:v>2.0833333333333332E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4</c:v>
+                  <c:v>2.0833333333333332E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4</c:v>
+                  <c:v>2.0833333333333332E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>14</c:v>
+                  <c:v>7.2916666666666671E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5</c:v>
+                  <c:v>2.6041666666666668E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>16</c:v>
+                  <c:v>8.3333333333333329E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>19</c:v>
+                  <c:v>9.8958333333333329E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>26</c:v>
+                  <c:v>0.13541666666666666</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>16</c:v>
+                  <c:v>8.3333333333333329E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9</c:v>
+                  <c:v>4.6875E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>10</c:v>
+                  <c:v>5.2083333333333336E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5</c:v>
+                  <c:v>2.6041666666666668E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6</c:v>
+                  <c:v>3.125E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.5625E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5038,7 +5423,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -5047,6 +5432,7 @@
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:tickLblSkip val="4"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
@@ -5057,7 +5443,7 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -5066,10 +5452,6 @@
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -5115,10 +5497,28 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00C853"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF5722"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
           <c:dLbls>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
-            <c:showCatName val="0"/>
+            <c:showCatName val="1"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
@@ -5166,10 +5566,6 @@
         <c:firstSliceAng val="0"/>
       </c:pieChart>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -5221,8 +5617,8 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>733425</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
@@ -5402,8 +5798,8 @@
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1057275</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
@@ -5431,16 +5827,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>47624</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>561975</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5472,8 +5868,8 @@
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
@@ -5851,8 +6247,8 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
@@ -41698,7 +42094,7 @@
       <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>536</v>
       </c>
     </row>
@@ -41976,7 +42372,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42211,7 +42607,7 @@
       <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>536</v>
       </c>
     </row>
@@ -42370,7 +42766,7 @@
       <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>536</v>
       </c>
     </row>
@@ -42402,7 +42798,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42558,8 +42954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42662,7 +43058,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42847,7 +43243,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42900,20 +43296,20 @@
       <c r="A3" t="s">
         <v>517</v>
       </c>
-      <c r="B3" s="13">
+      <c r="B3" s="12">
         <v>190</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C3" s="12">
         <v>192</v>
       </c>
-      <c r="D3" s="13">
+      <c r="D3" s="12">
         <v>190</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="12">
         <v>192</v>
       </c>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13">
+      <c r="F3" s="12"/>
+      <c r="G3" s="12">
         <f>SUM(B3:F3)</f>
         <v>764</v>
       </c>
@@ -42961,7 +43357,7 @@
       <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>536</v>
       </c>
     </row>
@@ -43097,7 +43493,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43220,7 +43616,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43342,8 +43738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43488,7 +43884,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="R22" sqref="R22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43909,7 +44305,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44038,7 +44434,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44299,7 +44695,7 @@
   <dimension ref="A1:W6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U9" sqref="U9"/>
+      <selection activeCell="S26" sqref="S26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44310,88 +44706,88 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B1" s="12">
+      <c r="B1" s="14">
         <v>0</v>
       </c>
-      <c r="C1" s="12">
-        <f>B1+5</f>
+      <c r="C1" s="14">
+        <f>B1+0.5</f>
+        <v>0.5</v>
+      </c>
+      <c r="D1" s="14">
+        <f t="shared" ref="D1:V1" si="0">C1+0.5</f>
+        <v>1</v>
+      </c>
+      <c r="E1" s="14">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="F1" s="14">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G1" s="14">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="H1" s="14">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="I1" s="14">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+      <c r="J1" s="14">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="K1" s="14">
+        <f t="shared" si="0"/>
+        <v>4.5</v>
+      </c>
+      <c r="L1" s="14">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="D1" s="12">
-        <f t="shared" ref="D1:V1" si="0">C1+5</f>
+      <c r="M1" s="14">
+        <f t="shared" si="0"/>
+        <v>5.5</v>
+      </c>
+      <c r="N1" s="14">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="O1" s="14">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="P1" s="14">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="Q1" s="14">
+        <f t="shared" si="0"/>
+        <v>7.5</v>
+      </c>
+      <c r="R1" s="14">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="S1" s="14">
+        <f t="shared" si="0"/>
+        <v>8.5</v>
+      </c>
+      <c r="T1" s="14">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="U1" s="14">
+        <f t="shared" si="0"/>
+        <v>9.5</v>
+      </c>
+      <c r="V1" s="14">
+        <f t="shared" si="0"/>
         <v>10</v>
-      </c>
-      <c r="E1" s="12">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="F1" s="12">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="G1" s="12">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="H1" s="12">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="I1" s="12">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-      <c r="J1" s="12">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="K1" s="12">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="L1" s="12">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="M1" s="12">
-        <f>L1+5</f>
-        <v>55</v>
-      </c>
-      <c r="N1" s="12">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-      <c r="O1" s="12">
-        <f t="shared" si="0"/>
-        <v>65</v>
-      </c>
-      <c r="P1" s="12">
-        <f t="shared" si="0"/>
-        <v>70</v>
-      </c>
-      <c r="Q1" s="12">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
-      <c r="R1" s="12">
-        <f t="shared" si="0"/>
-        <v>80</v>
-      </c>
-      <c r="S1" s="12">
-        <f t="shared" si="0"/>
-        <v>85</v>
-      </c>
-      <c r="T1" s="12">
-        <f t="shared" si="0"/>
-        <v>90</v>
-      </c>
-      <c r="U1" s="12">
-        <f>T1+5</f>
-        <v>95</v>
-      </c>
-      <c r="V1" s="12">
-        <f t="shared" si="0"/>
-        <v>100</v>
       </c>
       <c r="W1" t="s">
         <v>519</v>
@@ -44661,6 +45057,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update der Ergebnisse von Umfrage I
</commit_message>
<xml_diff>
--- a/documents/marketing/Umfrage-I Ergebnisse 21.12.2014.xlsx
+++ b/documents/marketing/Umfrage-I Ergebnisse 21.12.2014.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="315" windowWidth="23475" windowHeight="9765" tabRatio="728" firstSheet="1" activeTab="25"/>
+    <workbookView xWindow="360" yWindow="315" windowWidth="23475" windowHeight="9765" tabRatio="728" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Alle Ergebnisse" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
     <sheet name="Q25" sheetId="27" r:id="rId26"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Alle Ergebnisse'!$A$1:$CE$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Alle Ergebnisse'!$A$1:$CE$232</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -2457,19 +2457,19 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.1038961038961039</c:v>
+                  <c:v>0.1111111111111111</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.54978354978354982</c:v>
+                  <c:v>0.53240740740740744</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.27705627705627706</c:v>
+                  <c:v>0.28240740740740738</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.1948051948051951E-2</c:v>
+                  <c:v>5.5555555555555552E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.7316017316017316E-2</c:v>
+                  <c:v>1.8518518518518517E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2484,11 +2484,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="153503232"/>
-        <c:axId val="153504768"/>
+        <c:axId val="165652352"/>
+        <c:axId val="165653888"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="153503232"/>
+        <c:axId val="165652352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2497,14 +2497,15 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153504768"/>
+        <c:crossAx val="165653888"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="153504768"/>
+        <c:axId val="165653888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2515,7 +2516,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153503232"/>
+        <c:crossAx val="165652352"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
@@ -2632,11 +2634,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="183245824"/>
-        <c:axId val="183247616"/>
+        <c:axId val="142547584"/>
+        <c:axId val="142598528"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="183245824"/>
+        <c:axId val="142547584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2645,7 +2647,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="183247616"/>
+        <c:crossAx val="142598528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2653,7 +2655,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="183247616"/>
+        <c:axId val="142598528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2664,7 +2666,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="183245824"/>
+        <c:crossAx val="142547584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2782,11 +2784,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="190228352"/>
-        <c:axId val="190229504"/>
+        <c:axId val="182268288"/>
+        <c:axId val="182269824"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="190228352"/>
+        <c:axId val="182268288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2795,14 +2797,15 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="190229504"/>
+        <c:crossAx val="182269824"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="190229504"/>
+        <c:axId val="182269824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2813,7 +2816,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="190228352"/>
+        <c:crossAx val="182268288"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
@@ -3302,11 +3306,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="143946112"/>
-        <c:axId val="143947648"/>
+        <c:axId val="142863360"/>
+        <c:axId val="142869248"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="143946112"/>
+        <c:axId val="142863360"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3315,7 +3319,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143947648"/>
+        <c:crossAx val="142869248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3323,7 +3327,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="143947648"/>
+        <c:axId val="142869248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3334,7 +3338,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143946112"/>
+        <c:crossAx val="142863360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3482,11 +3486,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="144030336"/>
-        <c:axId val="144036224"/>
+        <c:axId val="142926976"/>
+        <c:axId val="142928512"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="144030336"/>
+        <c:axId val="142926976"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3495,7 +3499,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144036224"/>
+        <c:crossAx val="142928512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3503,7 +3507,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="144036224"/>
+        <c:axId val="142928512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3514,7 +3518,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144030336"/>
+        <c:crossAx val="142926976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3672,11 +3676,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="144245504"/>
-        <c:axId val="144247040"/>
+        <c:axId val="143015936"/>
+        <c:axId val="143017472"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="144245504"/>
+        <c:axId val="143015936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3695,7 +3699,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="144247040"/>
+        <c:crossAx val="143017472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3703,7 +3707,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="144247040"/>
+        <c:axId val="143017472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3714,7 +3718,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144245504"/>
+        <c:crossAx val="143015936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3946,11 +3950,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="16935936"/>
-        <c:axId val="156020736"/>
+        <c:axId val="143397632"/>
+        <c:axId val="143399168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="16935936"/>
+        <c:axId val="143397632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3959,14 +3963,15 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="156020736"/>
+        <c:crossAx val="143399168"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="156020736"/>
+        <c:axId val="143399168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3977,7 +3982,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="16935936"/>
+        <c:crossAx val="143397632"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
@@ -4112,11 +4118,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="182309632"/>
-        <c:axId val="182311168"/>
+        <c:axId val="181833088"/>
+        <c:axId val="181859456"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="182309632"/>
+        <c:axId val="181833088"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -4125,7 +4131,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="182311168"/>
+        <c:crossAx val="181859456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4133,7 +4139,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="182311168"/>
+        <c:axId val="181859456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4144,7 +4150,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="182309632"/>
+        <c:crossAx val="181833088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4262,11 +4268,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="156318720"/>
-        <c:axId val="183636736"/>
+        <c:axId val="143468800"/>
+        <c:axId val="143478784"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="156318720"/>
+        <c:axId val="143468800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4275,14 +4281,15 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="183636736"/>
+        <c:crossAx val="143478784"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="183636736"/>
+        <c:axId val="143478784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4293,7 +4300,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="156318720"/>
+        <c:crossAx val="143468800"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
@@ -4422,11 +4430,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="192124800"/>
-        <c:axId val="192126336"/>
+        <c:axId val="143494528"/>
+        <c:axId val="143512704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="192124800"/>
+        <c:axId val="143494528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4435,14 +4443,15 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="192126336"/>
+        <c:crossAx val="143512704"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="192126336"/>
+        <c:axId val="143512704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4453,7 +4462,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="192124800"/>
+        <c:crossAx val="143494528"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
@@ -4582,11 +4592,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="182626944"/>
-        <c:axId val="182649216"/>
+        <c:axId val="182191232"/>
+        <c:axId val="182192768"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="182626944"/>
+        <c:axId val="182191232"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -4595,7 +4605,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="182649216"/>
+        <c:crossAx val="182192768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4603,7 +4613,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="182649216"/>
+        <c:axId val="182192768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -4615,7 +4625,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="182626944"/>
+        <c:crossAx val="182191232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4733,11 +4743,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="184931840"/>
-        <c:axId val="184933376"/>
+        <c:axId val="182209152"/>
+        <c:axId val="182223232"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="184931840"/>
+        <c:axId val="182209152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4746,14 +4756,15 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="184933376"/>
+        <c:crossAx val="182223232"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="184933376"/>
+        <c:axId val="182223232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.70000000000000007"/>
@@ -4765,7 +4776,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="184931840"/>
+        <c:crossAx val="182209152"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
@@ -4888,11 +4900,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="132610688"/>
-        <c:axId val="187832192"/>
+        <c:axId val="182318592"/>
+        <c:axId val="182320128"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="132610688"/>
+        <c:axId val="182318592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4901,14 +4913,15 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="187832192"/>
+        <c:crossAx val="182320128"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="187832192"/>
+        <c:axId val="182320128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.5"/>
@@ -4920,7 +4933,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132610688"/>
+        <c:crossAx val="182318592"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
@@ -5055,11 +5069,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="182785920"/>
-        <c:axId val="182787456"/>
+        <c:axId val="182332416"/>
+        <c:axId val="182358784"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="182785920"/>
+        <c:axId val="182332416"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -5068,7 +5082,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="182787456"/>
+        <c:crossAx val="182358784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5076,7 +5090,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="182787456"/>
+        <c:axId val="182358784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5087,7 +5101,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="182785920"/>
+        <c:crossAx val="182332416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5413,11 +5427,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="182827264"/>
-        <c:axId val="182837248"/>
+        <c:axId val="182041216"/>
+        <c:axId val="142221696"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="182827264"/>
+        <c:axId val="182041216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5427,7 +5441,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="182837248"/>
+        <c:crossAx val="142221696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5436,7 +5450,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="182837248"/>
+        <c:axId val="142221696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5447,7 +5461,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="182827264"/>
+        <c:crossAx val="182041216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6602,8 +6616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CE232"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView showGridLines="0" topLeftCell="BN1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="CI175" sqref="CI175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14342,7 +14356,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="50" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:83" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>15519639</v>
       </c>
@@ -16719,7 +16733,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="65" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:83" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A65" s="5">
         <v>15520784</v>
       </c>
@@ -19331,7 +19345,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="83" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:83" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A83" s="5">
         <v>15522996</v>
       </c>
@@ -19623,7 +19637,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="85" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:83" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A85" s="5">
         <v>15523173</v>
       </c>
@@ -23003,7 +23017,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="107" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:83" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A107" s="5">
         <v>15526098</v>
       </c>
@@ -25806,7 +25820,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="126" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:83" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A126" s="5">
         <v>15533646</v>
       </c>
@@ -29442,7 +29456,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="150" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:83" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A150" s="5">
         <v>15544632</v>
       </c>
@@ -30601,7 +30615,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="159" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:83" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A159" s="5">
         <v>15547636</v>
       </c>
@@ -39159,7 +39173,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="215" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:83" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A215" s="5">
         <v>15613387</v>
       </c>
@@ -40381,7 +40395,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="223" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:83" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A223" s="5">
         <v>15619124</v>
       </c>
@@ -41956,7 +41970,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:CE1"/>
+  <autoFilter ref="A1:CE232"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
@@ -41966,7 +41980,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -42955,7 +42969,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42994,10 +43008,10 @@
         <v>24</v>
       </c>
       <c r="C2">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="D2">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E2">
         <v>12</v>
@@ -43007,7 +43021,7 @@
       </c>
       <c r="G2">
         <f>SUM(B2:F2)</f>
-        <v>231</v>
+        <v>216</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -43016,23 +43030,23 @@
       </c>
       <c r="B3" s="8">
         <f>B2/$G$2</f>
-        <v>0.1038961038961039</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="C3" s="8">
         <f t="shared" ref="C3:F3" si="0">C2/$G$2</f>
-        <v>0.54978354978354982</v>
+        <v>0.53240740740740744</v>
       </c>
       <c r="D3" s="8">
         <f t="shared" si="0"/>
-        <v>0.27705627705627706</v>
+        <v>0.28240740740740738</v>
       </c>
       <c r="E3" s="8">
         <f t="shared" si="0"/>
-        <v>5.1948051948051951E-2</v>
+        <v>5.5555555555555552E-2</v>
       </c>
       <c r="F3" s="8">
         <f t="shared" si="0"/>
-        <v>1.7316017316017316E-2</v>
+        <v>1.8518518518518517E-2</v>
       </c>
       <c r="G3" s="8">
         <f>SUM(B3:F3)</f>
@@ -43738,7 +43752,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Analyse von Umfrage I abgeschlossen
</commit_message>
<xml_diff>
--- a/documents/marketing/Umfrage-I Ergebnisse 21.12.2014.xlsx
+++ b/documents/marketing/Umfrage-I Ergebnisse 21.12.2014.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="315" windowWidth="23475" windowHeight="9765" tabRatio="728" activeTab="9"/>
+    <workbookView xWindow="360" yWindow="315" windowWidth="23475" windowHeight="9765" tabRatio="728" firstSheet="3" activeTab="26"/>
   </bookViews>
   <sheets>
     <sheet name="Alle Ergebnisse" sheetId="1" r:id="rId1"/>
@@ -33,6 +33,8 @@
     <sheet name="Q23" sheetId="25" r:id="rId24"/>
     <sheet name="Q24" sheetId="26" r:id="rId25"/>
     <sheet name="Q25" sheetId="27" r:id="rId26"/>
+    <sheet name="Q16--Q9" sheetId="28" r:id="rId27"/>
+    <sheet name="Q14--Q9" sheetId="29" r:id="rId28"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Alle Ergebnisse'!$A$1:$CE$232</definedName>
@@ -76,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3460" uniqueCount="548">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3514" uniqueCount="551">
   <si>
     <t>_Antwort-ID</t>
   </si>
@@ -1720,6 +1722,15 @@
   </si>
   <si>
     <t>Mittelwert</t>
+  </si>
+  <si>
+    <t>Q9</t>
+  </si>
+  <si>
+    <t>Q16</t>
+  </si>
+  <si>
+    <t>Q14</t>
   </si>
 </sst>
 </file>
@@ -1903,7 +1914,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2089,6 +2100,36 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF5722"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF50057"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -2221,7 +2262,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -2264,8 +2305,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2299,8 +2341,33 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="34" borderId="0" xfId="42" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="35" borderId="0" xfId="42" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="36" borderId="0" xfId="42" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="37" borderId="0" xfId="42" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="38" borderId="0" xfId="42" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -2333,6 +2400,7 @@
     <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Prozent" xfId="42" builtinId="5"/>
     <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
@@ -2350,8 +2418,8 @@
     <mruColors>
       <color rgb="FFFF5722"/>
       <color rgb="FF00C853"/>
+      <color rgb="FFF50057"/>
       <color rgb="FF3F51B5"/>
-      <color rgb="FFF50057"/>
     </mruColors>
   </colors>
   <extLst>
@@ -2484,11 +2552,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="165652352"/>
-        <c:axId val="165653888"/>
+        <c:axId val="148940672"/>
+        <c:axId val="148942208"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="165652352"/>
+        <c:axId val="148940672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2497,7 +2565,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="165653888"/>
+        <c:crossAx val="148942208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2505,7 +2573,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="165653888"/>
+        <c:axId val="148942208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2516,7 +2584,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="165652352"/>
+        <c:crossAx val="148940672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2634,11 +2702,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="142547584"/>
-        <c:axId val="142598528"/>
+        <c:axId val="150874752"/>
+        <c:axId val="150888832"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="142547584"/>
+        <c:axId val="150874752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2647,7 +2715,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142598528"/>
+        <c:crossAx val="150888832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2655,7 +2723,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="142598528"/>
+        <c:axId val="150888832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2666,7 +2734,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142547584"/>
+        <c:crossAx val="150874752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2784,11 +2852,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="182268288"/>
-        <c:axId val="182269824"/>
+        <c:axId val="150925696"/>
+        <c:axId val="150927232"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="182268288"/>
+        <c:axId val="150925696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2797,7 +2865,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="182269824"/>
+        <c:crossAx val="150927232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2805,7 +2873,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="182269824"/>
+        <c:axId val="150927232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2816,7 +2884,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="182268288"/>
+        <c:crossAx val="150925696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3306,11 +3374,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="142863360"/>
-        <c:axId val="142869248"/>
+        <c:axId val="150793216"/>
+        <c:axId val="185205504"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="142863360"/>
+        <c:axId val="150793216"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3319,7 +3387,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142869248"/>
+        <c:crossAx val="185205504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3327,7 +3395,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="142869248"/>
+        <c:axId val="185205504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3338,7 +3406,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142863360"/>
+        <c:crossAx val="150793216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3486,11 +3554,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="142926976"/>
-        <c:axId val="142928512"/>
+        <c:axId val="185263232"/>
+        <c:axId val="185264768"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="142926976"/>
+        <c:axId val="185263232"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3499,7 +3567,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142928512"/>
+        <c:crossAx val="185264768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3507,7 +3575,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="142928512"/>
+        <c:axId val="185264768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3518,7 +3586,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142926976"/>
+        <c:crossAx val="185263232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3676,11 +3744,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="143015936"/>
-        <c:axId val="143017472"/>
+        <c:axId val="185352192"/>
+        <c:axId val="185353728"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="143015936"/>
+        <c:axId val="185352192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3699,7 +3767,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="143017472"/>
+        <c:crossAx val="185353728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3707,7 +3775,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="143017472"/>
+        <c:axId val="185353728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3718,7 +3786,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143015936"/>
+        <c:crossAx val="185352192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3950,11 +4018,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="143397632"/>
-        <c:axId val="143399168"/>
+        <c:axId val="185733888"/>
+        <c:axId val="185735424"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="143397632"/>
+        <c:axId val="185733888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3963,7 +4031,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143399168"/>
+        <c:crossAx val="185735424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3971,7 +4039,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="143399168"/>
+        <c:axId val="185735424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3982,7 +4050,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143397632"/>
+        <c:crossAx val="185733888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4118,11 +4186,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="181833088"/>
-        <c:axId val="181859456"/>
+        <c:axId val="149982592"/>
+        <c:axId val="150008960"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="181833088"/>
+        <c:axId val="149982592"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -4131,7 +4199,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="181859456"/>
+        <c:crossAx val="150008960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4139,7 +4207,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="181859456"/>
+        <c:axId val="150008960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4150,7 +4218,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="181833088"/>
+        <c:crossAx val="149982592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4268,11 +4336,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="143468800"/>
-        <c:axId val="143478784"/>
+        <c:axId val="186198272"/>
+        <c:axId val="186208256"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="143468800"/>
+        <c:axId val="186198272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4281,7 +4349,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143478784"/>
+        <c:crossAx val="186208256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4289,7 +4357,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="143478784"/>
+        <c:axId val="186208256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4300,7 +4368,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143468800"/>
+        <c:crossAx val="186198272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4430,11 +4498,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="143494528"/>
-        <c:axId val="143512704"/>
+        <c:axId val="186224000"/>
+        <c:axId val="186242176"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="143494528"/>
+        <c:axId val="186224000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4443,7 +4511,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143512704"/>
+        <c:crossAx val="186242176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4451,7 +4519,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="143512704"/>
+        <c:axId val="186242176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4462,11 +4530,443 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143494528"/>
+        <c:crossAx val="186224000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Q16--Q9'!$A$21:$B$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Q16 Ja</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="00C853"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'Q16--Q9'!$C$19:$D$20</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="2"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Ja</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Nein</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Q9</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Q16--Q9'!$C$21:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.56666666666666665</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.27160493827160492</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Q16--Q9'!$A$22:$B$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Q16 Nein</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF5722"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'Q16--Q9'!$C$19:$D$20</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="2"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Ja</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Nein</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Q9</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Q16--Q9'!$C$22:$D$22</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.43333333333333335</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.72839506172839508</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="156772608"/>
+        <c:axId val="156786688"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="156772608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="156786688"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="156786688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="156772608"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Q14--Q9'!$A$21:$B$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Q14 Ja</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="00C853"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'Q14--Q9'!$C$19:$D$20</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="2"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Ja</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Nein</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Q9</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Q14--Q9'!$C$21:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.8666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.78395061728395066</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Q14--Q9'!$A$22:$B$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Q14 Nein</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF5722"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'Q14--Q9'!$C$19:$D$20</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="2"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Ja</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Nein</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Q9</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Q14--Q9'!$C$22:$D$22</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.13333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.21604938271604937</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="169808256"/>
+        <c:axId val="169810944"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="169808256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="169810944"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="169810944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="169808256"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -4592,11 +5092,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="182191232"/>
-        <c:axId val="182192768"/>
+        <c:axId val="150340736"/>
+        <c:axId val="150342272"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="182191232"/>
+        <c:axId val="150340736"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -4605,7 +5105,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="182192768"/>
+        <c:crossAx val="150342272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4613,7 +5113,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="182192768"/>
+        <c:axId val="150342272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -4625,7 +5125,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="182191232"/>
+        <c:crossAx val="150340736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4743,11 +5243,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="182209152"/>
-        <c:axId val="182223232"/>
+        <c:axId val="150358656"/>
+        <c:axId val="150372736"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="182209152"/>
+        <c:axId val="150358656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4756,7 +5256,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="182223232"/>
+        <c:crossAx val="150372736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4764,7 +5264,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="182223232"/>
+        <c:axId val="150372736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.70000000000000007"/>
@@ -4776,7 +5276,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="182209152"/>
+        <c:crossAx val="150358656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4900,11 +5400,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="182318592"/>
-        <c:axId val="182320128"/>
+        <c:axId val="150466944"/>
+        <c:axId val="150468480"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="182318592"/>
+        <c:axId val="150466944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4913,7 +5413,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="182320128"/>
+        <c:crossAx val="150468480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4921,7 +5421,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="182320128"/>
+        <c:axId val="150468480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.5"/>
@@ -4933,7 +5433,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="182318592"/>
+        <c:crossAx val="150466944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5069,11 +5569,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="182332416"/>
-        <c:axId val="182358784"/>
+        <c:axId val="150480768"/>
+        <c:axId val="150482304"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="182332416"/>
+        <c:axId val="150480768"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -5082,7 +5582,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="182358784"/>
+        <c:crossAx val="150482304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5090,7 +5590,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="182358784"/>
+        <c:axId val="150482304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5101,7 +5601,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="182332416"/>
+        <c:crossAx val="150480768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5427,11 +5927,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="182041216"/>
-        <c:axId val="142221696"/>
+        <c:axId val="150518400"/>
+        <c:axId val="150806912"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="182041216"/>
+        <c:axId val="150518400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5441,7 +5941,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142221696"/>
+        <c:crossAx val="150806912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5450,7 +5950,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="142221696"/>
+        <c:axId val="150806912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5461,7 +5961,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="182041216"/>
+        <c:crossAx val="150518400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6077,6 +6577,156 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing22.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>733425</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>685044</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>180267</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Grafik 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9410700" y="228600"/>
+          <a:ext cx="6047619" cy="5666667"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Diagramm 6"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing23.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Diagramm 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>142115</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>180324</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Grafik 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8839200" y="304800"/>
+          <a:ext cx="6076190" cy="5209524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -14356,7 +15006,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="50" spans="1:83" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>15519639</v>
       </c>
@@ -16733,7 +17383,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="65" spans="1:83" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A65" s="5">
         <v>15520784</v>
       </c>
@@ -19345,7 +19995,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="83" spans="1:83" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A83" s="5">
         <v>15522996</v>
       </c>
@@ -19637,7 +20287,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="85" spans="1:83" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A85" s="5">
         <v>15523173</v>
       </c>
@@ -23017,7 +23667,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="107" spans="1:83" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A107" s="5">
         <v>15526098</v>
       </c>
@@ -25820,7 +26470,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="126" spans="1:83" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A126" s="5">
         <v>15533646</v>
       </c>
@@ -29456,7 +30106,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="150" spans="1:83" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A150" s="5">
         <v>15544632</v>
       </c>
@@ -30615,7 +31265,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="159" spans="1:83" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A159" s="5">
         <v>15547636</v>
       </c>
@@ -39173,7 +39823,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="215" spans="1:83" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A215" s="5">
         <v>15613387</v>
       </c>
@@ -40395,7 +41045,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="223" spans="1:83" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A223" s="5">
         <v>15619124</v>
       </c>
@@ -41980,7 +42630,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -43893,6 +44543,671 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="6.7109375" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" customWidth="1"/>
+    <col min="5" max="5" width="6.140625" customWidth="1"/>
+    <col min="6" max="6" width="6" customWidth="1"/>
+    <col min="7" max="7" width="6.42578125" customWidth="1"/>
+    <col min="8" max="8" width="6.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C1" s="15" t="s">
+        <v>548</v>
+      </c>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15" t="s">
+        <v>519</v>
+      </c>
+      <c r="H1" s="15"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C2" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="F2" s="15"/>
+      <c r="G2" s="17" t="s">
+        <v>517</v>
+      </c>
+      <c r="H2" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>549</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3">
+        <v>17</v>
+      </c>
+      <c r="D3" s="21">
+        <f>C3/G3</f>
+        <v>0.27868852459016391</v>
+      </c>
+      <c r="E3">
+        <v>44</v>
+      </c>
+      <c r="F3" s="21">
+        <f>E3/G3</f>
+        <v>0.72131147540983609</v>
+      </c>
+      <c r="G3" s="24">
+        <v>61</v>
+      </c>
+      <c r="H3" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="19">
+        <f>C3/C7</f>
+        <v>0.56666666666666665</v>
+      </c>
+      <c r="D4" s="22">
+        <f>C3/G7</f>
+        <v>8.8541666666666671E-2</v>
+      </c>
+      <c r="E4" s="20">
+        <f>E3/E7</f>
+        <v>0.27160493827160492</v>
+      </c>
+      <c r="F4" s="22">
+        <f>E3/G7</f>
+        <v>0.22916666666666666</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="16"/>
+      <c r="B5" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5">
+        <v>13</v>
+      </c>
+      <c r="D5" s="23">
+        <f>C5/G5</f>
+        <v>9.9236641221374045E-2</v>
+      </c>
+      <c r="E5">
+        <v>118</v>
+      </c>
+      <c r="F5" s="23">
+        <f>E5/G5</f>
+        <v>0.9007633587786259</v>
+      </c>
+      <c r="G5" s="26">
+        <v>131</v>
+      </c>
+      <c r="H5" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="16"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="19">
+        <f>C5/C7</f>
+        <v>0.43333333333333335</v>
+      </c>
+      <c r="D6" s="22">
+        <f>C5/G7</f>
+        <v>6.7708333333333329E-2</v>
+      </c>
+      <c r="E6" s="20">
+        <f>E5/E7</f>
+        <v>0.72839506172839508</v>
+      </c>
+      <c r="F6" s="22">
+        <f>E5/G7</f>
+        <v>0.61458333333333337</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>519</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>517</v>
+      </c>
+      <c r="C7" s="28">
+        <v>30</v>
+      </c>
+      <c r="E7" s="27">
+        <v>162</v>
+      </c>
+      <c r="G7" s="25">
+        <f>SUM(G3:G6)</f>
+        <v>192</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="16"/>
+      <c r="B8" t="s">
+        <v>518</v>
+      </c>
+      <c r="C8" s="19">
+        <v>1</v>
+      </c>
+      <c r="E8" s="20">
+        <v>1</v>
+      </c>
+      <c r="H8" s="30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C12" s="15" t="s">
+        <v>548</v>
+      </c>
+      <c r="D12" s="15"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" t="s">
+        <v>86</v>
+      </c>
+      <c r="E13" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>549</v>
+      </c>
+      <c r="B14" t="s">
+        <v>85</v>
+      </c>
+      <c r="C14">
+        <f>C3</f>
+        <v>17</v>
+      </c>
+      <c r="D14">
+        <f>E3</f>
+        <v>44</v>
+      </c>
+      <c r="E14">
+        <f>SUM(C14:D14)</f>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="16"/>
+      <c r="B15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15">
+        <f>C5</f>
+        <v>13</v>
+      </c>
+      <c r="D15">
+        <f>E5</f>
+        <v>118</v>
+      </c>
+      <c r="E15">
+        <f>SUM(C15:D15)</f>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>517</v>
+      </c>
+      <c r="C16">
+        <f>SUM(C14:C15)</f>
+        <v>30</v>
+      </c>
+      <c r="D16">
+        <f>SUM(D14:D15)</f>
+        <v>162</v>
+      </c>
+      <c r="E16">
+        <f>SUM(C16:D16)</f>
+        <v>192</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C19" s="15" t="s">
+        <v>548</v>
+      </c>
+      <c r="D19" s="15"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>534</v>
+      </c>
+      <c r="D20" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="16" t="s">
+        <v>549</v>
+      </c>
+      <c r="B21" t="s">
+        <v>534</v>
+      </c>
+      <c r="C21" s="31">
+        <f>C14/C16</f>
+        <v>0.56666666666666665</v>
+      </c>
+      <c r="D21" s="31">
+        <f>D14/D16</f>
+        <v>0.27160493827160492</v>
+      </c>
+      <c r="E21" s="18"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="16"/>
+      <c r="B22" t="s">
+        <v>535</v>
+      </c>
+      <c r="C22" s="31">
+        <f>C15/C16</f>
+        <v>0.43333333333333335</v>
+      </c>
+      <c r="D22" s="31">
+        <f>D15/D16</f>
+        <v>0.72839506172839508</v>
+      </c>
+      <c r="E22" s="18"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>518</v>
+      </c>
+      <c r="C23" s="29">
+        <f>C21+C22</f>
+        <v>1</v>
+      </c>
+      <c r="D23" s="29">
+        <f>D21+D22</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="6.7109375" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" customWidth="1"/>
+    <col min="5" max="5" width="6.140625" customWidth="1"/>
+    <col min="6" max="6" width="6" customWidth="1"/>
+    <col min="7" max="7" width="6.42578125" customWidth="1"/>
+    <col min="8" max="8" width="6.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C1" s="15" t="s">
+        <v>548</v>
+      </c>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15" t="s">
+        <v>519</v>
+      </c>
+      <c r="H1" s="15"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C2" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="F2" s="15"/>
+      <c r="G2" s="17" t="s">
+        <v>517</v>
+      </c>
+      <c r="H2" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>550</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3">
+        <v>26</v>
+      </c>
+      <c r="D3" s="21">
+        <f>C3/G3</f>
+        <v>0.42622950819672129</v>
+      </c>
+      <c r="E3">
+        <v>127</v>
+      </c>
+      <c r="F3" s="21">
+        <f>E3/G3</f>
+        <v>2.081967213114754</v>
+      </c>
+      <c r="G3" s="24">
+        <v>61</v>
+      </c>
+      <c r="H3" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="19">
+        <f>C3/C7</f>
+        <v>0.8666666666666667</v>
+      </c>
+      <c r="D4" s="22">
+        <f>C3/G7</f>
+        <v>0.13541666666666666</v>
+      </c>
+      <c r="E4" s="20">
+        <f>E3/E7</f>
+        <v>0.78395061728395066</v>
+      </c>
+      <c r="F4" s="22">
+        <f>E3/G7</f>
+        <v>0.66145833333333337</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="16"/>
+      <c r="B5" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5" s="23">
+        <f>C5/G5</f>
+        <v>3.0534351145038167E-2</v>
+      </c>
+      <c r="E5">
+        <v>35</v>
+      </c>
+      <c r="F5" s="23">
+        <f>E5/G5</f>
+        <v>0.26717557251908397</v>
+      </c>
+      <c r="G5" s="26">
+        <v>131</v>
+      </c>
+      <c r="H5" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="16"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="19">
+        <f>C5/C7</f>
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="D6" s="22">
+        <f>C5/G7</f>
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="E6" s="20">
+        <f>E5/E7</f>
+        <v>0.21604938271604937</v>
+      </c>
+      <c r="F6" s="22">
+        <f>E5/G7</f>
+        <v>0.18229166666666666</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>519</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>517</v>
+      </c>
+      <c r="C7" s="28">
+        <v>30</v>
+      </c>
+      <c r="E7" s="27">
+        <v>162</v>
+      </c>
+      <c r="G7" s="25">
+        <f>SUM(G3:G6)</f>
+        <v>192</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="16"/>
+      <c r="B8" t="s">
+        <v>518</v>
+      </c>
+      <c r="C8" s="19">
+        <v>1</v>
+      </c>
+      <c r="E8" s="20">
+        <v>1</v>
+      </c>
+      <c r="H8" s="30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C12" s="15" t="s">
+        <v>548</v>
+      </c>
+      <c r="D12" s="15"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" t="s">
+        <v>86</v>
+      </c>
+      <c r="E13" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>550</v>
+      </c>
+      <c r="B14" t="s">
+        <v>85</v>
+      </c>
+      <c r="C14">
+        <f>C3</f>
+        <v>26</v>
+      </c>
+      <c r="D14">
+        <f>E3</f>
+        <v>127</v>
+      </c>
+      <c r="E14">
+        <f>SUM(C14:D14)</f>
+        <v>153</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="16"/>
+      <c r="B15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15">
+        <f>C5</f>
+        <v>4</v>
+      </c>
+      <c r="D15">
+        <f>E5</f>
+        <v>35</v>
+      </c>
+      <c r="E15">
+        <f>SUM(C15:D15)</f>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>517</v>
+      </c>
+      <c r="C16">
+        <f>SUM(C14:C15)</f>
+        <v>30</v>
+      </c>
+      <c r="D16">
+        <f>SUM(D14:D15)</f>
+        <v>162</v>
+      </c>
+      <c r="E16">
+        <f>SUM(C16:D16)</f>
+        <v>192</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C19" s="15" t="s">
+        <v>548</v>
+      </c>
+      <c r="D19" s="15"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>534</v>
+      </c>
+      <c r="D20" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="16" t="s">
+        <v>550</v>
+      </c>
+      <c r="B21" t="s">
+        <v>534</v>
+      </c>
+      <c r="C21" s="31">
+        <f>C14/C16</f>
+        <v>0.8666666666666667</v>
+      </c>
+      <c r="D21" s="31">
+        <f>D14/D16</f>
+        <v>0.78395061728395066</v>
+      </c>
+      <c r="E21" s="18"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="16"/>
+      <c r="B22" t="s">
+        <v>535</v>
+      </c>
+      <c r="C22" s="31">
+        <f>C15/C16</f>
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="D22" s="31">
+        <f>D15/D16</f>
+        <v>0.21604938271604937</v>
+      </c>
+      <c r="E22" s="18"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>518</v>
+      </c>
+      <c r="C23" s="29">
+        <f>C21+C22</f>
+        <v>1</v>
+      </c>
+      <c r="D23" s="29">
+        <f>D21+D22</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I6"/>

</xml_diff>

<commit_message>
Exceldaten und Grafiken aktualisiert
</commit_message>
<xml_diff>
--- a/documents/marketing/Umfrage-I Ergebnisse 21.12.2014.xlsx
+++ b/documents/marketing/Umfrage-I Ergebnisse 21.12.2014.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="315" windowWidth="23475" windowHeight="9765" tabRatio="728" firstSheet="3" activeTab="26"/>
+    <workbookView xWindow="360" yWindow="315" windowWidth="23475" windowHeight="9765" tabRatio="765" firstSheet="14" activeTab="33"/>
   </bookViews>
   <sheets>
     <sheet name="Alle Ergebnisse" sheetId="1" r:id="rId1"/>
@@ -35,6 +35,12 @@
     <sheet name="Q25" sheetId="27" r:id="rId26"/>
     <sheet name="Q16--Q9" sheetId="28" r:id="rId27"/>
     <sheet name="Q14--Q9" sheetId="29" r:id="rId28"/>
+    <sheet name="Q18e--Q4" sheetId="30" r:id="rId29"/>
+    <sheet name="Q18e--Q7" sheetId="32" r:id="rId30"/>
+    <sheet name="Q18e--Q9" sheetId="33" r:id="rId31"/>
+    <sheet name="Q18e--Q13" sheetId="34" r:id="rId32"/>
+    <sheet name="Q18e--Q14" sheetId="36" r:id="rId33"/>
+    <sheet name="Q18e--Q16" sheetId="37" r:id="rId34"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Alle Ergebnisse'!$A$1:$CE$232</definedName>
@@ -78,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3514" uniqueCount="551">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3626" uniqueCount="555">
   <si>
     <t>_Antwort-ID</t>
   </si>
@@ -1731,6 +1737,18 @@
   </si>
   <si>
     <t>Q14</t>
+  </si>
+  <si>
+    <t>Q18e</t>
+  </si>
+  <si>
+    <t>Q4</t>
+  </si>
+  <si>
+    <t>Q7</t>
+  </si>
+  <si>
+    <t>Q13</t>
   </si>
 </sst>
 </file>
@@ -2307,7 +2325,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2342,9 +2360,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -2366,6 +2381,33 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2416,9 +2458,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
-      <color rgb="FFFF5722"/>
       <color rgb="FF00C853"/>
       <color rgb="FFF50057"/>
+      <color rgb="FFFF5722"/>
       <color rgb="FF3F51B5"/>
     </mruColors>
   </colors>
@@ -2552,11 +2594,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="148940672"/>
-        <c:axId val="148942208"/>
+        <c:axId val="89053824"/>
+        <c:axId val="89014656"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="148940672"/>
+        <c:axId val="89053824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2565,7 +2607,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148942208"/>
+        <c:crossAx val="89014656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2573,7 +2615,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="148942208"/>
+        <c:axId val="89014656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2584,7 +2626,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148940672"/>
+        <c:crossAx val="89053824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2702,11 +2744,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="150874752"/>
-        <c:axId val="150888832"/>
+        <c:axId val="75197824"/>
+        <c:axId val="75211904"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="150874752"/>
+        <c:axId val="75197824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2715,7 +2757,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="150888832"/>
+        <c:crossAx val="75211904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2723,7 +2765,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="150888832"/>
+        <c:axId val="75211904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2734,7 +2776,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="150874752"/>
+        <c:crossAx val="75197824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2852,11 +2894,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="150925696"/>
-        <c:axId val="150927232"/>
+        <c:axId val="75236480"/>
+        <c:axId val="75238016"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="150925696"/>
+        <c:axId val="75236480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2865,7 +2907,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="150927232"/>
+        <c:crossAx val="75238016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2873,7 +2915,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="150927232"/>
+        <c:axId val="75238016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2884,7 +2926,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="150925696"/>
+        <c:crossAx val="75236480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3374,11 +3416,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="150793216"/>
-        <c:axId val="185205504"/>
+        <c:axId val="75628544"/>
+        <c:axId val="75630080"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="150793216"/>
+        <c:axId val="75628544"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3387,7 +3429,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="185205504"/>
+        <c:crossAx val="75630080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3395,7 +3437,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="185205504"/>
+        <c:axId val="75630080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3406,7 +3448,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="150793216"/>
+        <c:crossAx val="75628544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3554,11 +3596,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="185263232"/>
-        <c:axId val="185264768"/>
+        <c:axId val="76052352"/>
+        <c:axId val="76053888"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="185263232"/>
+        <c:axId val="76052352"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -3567,7 +3609,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="185264768"/>
+        <c:crossAx val="76053888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3575,7 +3617,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="185264768"/>
+        <c:axId val="76053888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3586,7 +3628,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="185263232"/>
+        <c:crossAx val="76052352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3744,11 +3786,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="185352192"/>
-        <c:axId val="185353728"/>
+        <c:axId val="75784960"/>
+        <c:axId val="75786496"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="185352192"/>
+        <c:axId val="75784960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3767,7 +3809,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="185353728"/>
+        <c:crossAx val="75786496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3775,7 +3817,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="185353728"/>
+        <c:axId val="75786496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3786,7 +3828,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="185352192"/>
+        <c:crossAx val="75784960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4018,11 +4060,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="185733888"/>
-        <c:axId val="185735424"/>
+        <c:axId val="76162560"/>
+        <c:axId val="76164096"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="185733888"/>
+        <c:axId val="76162560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4031,7 +4073,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="185735424"/>
+        <c:crossAx val="76164096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4039,7 +4081,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="185735424"/>
+        <c:axId val="76164096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4050,7 +4092,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="185733888"/>
+        <c:crossAx val="76162560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4186,11 +4228,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="149982592"/>
-        <c:axId val="150008960"/>
+        <c:axId val="104374656"/>
+        <c:axId val="104376192"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="149982592"/>
+        <c:axId val="104374656"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -4199,7 +4241,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="150008960"/>
+        <c:crossAx val="104376192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4207,7 +4249,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="150008960"/>
+        <c:axId val="104376192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4218,7 +4260,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149982592"/>
+        <c:crossAx val="104374656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4336,11 +4378,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="186198272"/>
-        <c:axId val="186208256"/>
+        <c:axId val="76372992"/>
+        <c:axId val="76374784"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="186198272"/>
+        <c:axId val="76372992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4349,7 +4391,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="186208256"/>
+        <c:crossAx val="76374784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4357,7 +4399,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="186208256"/>
+        <c:axId val="76374784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4368,7 +4410,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="186198272"/>
+        <c:crossAx val="76372992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4498,11 +4540,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="186224000"/>
-        <c:axId val="186242176"/>
+        <c:axId val="76411264"/>
+        <c:axId val="76412800"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="186224000"/>
+        <c:axId val="76411264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4511,7 +4553,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="186242176"/>
+        <c:crossAx val="76412800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4519,7 +4561,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="186242176"/>
+        <c:axId val="76412800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4530,7 +4572,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="186224000"/>
+        <c:crossAx val="76411264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4709,11 +4751,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="156772608"/>
-        <c:axId val="156786688"/>
+        <c:axId val="76492160"/>
+        <c:axId val="76498048"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="156772608"/>
+        <c:axId val="76492160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4722,7 +4764,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="156786688"/>
+        <c:crossAx val="76498048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4730,7 +4772,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="156786688"/>
+        <c:axId val="76498048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4741,7 +4783,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="156772608"/>
+        <c:crossAx val="76492160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4925,11 +4967,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="169808256"/>
-        <c:axId val="169810944"/>
+        <c:axId val="76552832"/>
+        <c:axId val="76562816"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="169808256"/>
+        <c:axId val="76552832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4938,7 +4980,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169810944"/>
+        <c:crossAx val="76562816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4946,7 +4988,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="169810944"/>
+        <c:axId val="76562816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4957,7 +4999,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="169808256"/>
+        <c:crossAx val="76552832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4967,6 +5009,781 @@
       <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Social Media</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="00C853"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Q18e--Q4'!$D$10:$G$10</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5-7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7&lt;</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Q18e--Q4'!$D$12:$G$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0" formatCode="0%">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.51549999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.44330000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.1200000000000001E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Gesamt</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF5722"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Q18e--Q4'!$D$10:$G$10</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5-7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7&lt;</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Q18e--Q4'!$D$13:$G$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.56770833333333337</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.38541666666666669</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.6875E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="56563584"/>
+        <c:axId val="56565120"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="56563584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="56565120"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="56565120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="56563584"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart25.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Q18e--Q7'!$B$12:$C$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Social Media %</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF5722"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00C853"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Q18e--Q7'!$D$10:$E$10</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>ja</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>nein</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Q18e--Q7'!$D$12:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.865979381443299</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.13402061855670103</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart26.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Q18e--Q9'!$B$12:$C$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Social Media %</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF5722"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00C853"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Q18e--Q9'!$D$10:$E$10</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>ja</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>nein</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Q18e--Q9'!$D$12:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.19587628865979381</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.80412371134020622</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart27.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Q18e--Q13'!$B$12:$C$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Social Media %</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF5722"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="F50057"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00C853"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Q18e--Q13'!$D$10:$F$10</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>ab und zu</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>ja</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>nein</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Q18e--Q13'!$D$12:$F$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.65979381443298968</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.26804123711340205</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.2164948453608241E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart28.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Q18e--Q14'!$B$12:$C$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Social Media %</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF5722"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00C853"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Q18e--Q14'!$D$10:$E$10</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>ja</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>nein</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Q18e--Q14'!$D$12:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.88659793814432986</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1134020618556701</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart29.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Q18e--Q16'!$B$12:$C$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Social Media %</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF5722"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00C853"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Q18e--Q16'!$D$10:$E$10</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>ja</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>nein</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Q18e--Q16'!$D$12:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.35051546391752575</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.64948453608247425</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -5092,11 +5909,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="150340736"/>
-        <c:axId val="150342272"/>
+        <c:axId val="74913664"/>
+        <c:axId val="74915200"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="150340736"/>
+        <c:axId val="74913664"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -5105,7 +5922,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="150342272"/>
+        <c:crossAx val="74915200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5113,7 +5930,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="150342272"/>
+        <c:axId val="74915200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -5125,7 +5942,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="150340736"/>
+        <c:crossAx val="74913664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5243,11 +6060,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="150358656"/>
-        <c:axId val="150372736"/>
+        <c:axId val="74935680"/>
+        <c:axId val="74970240"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="150358656"/>
+        <c:axId val="74935680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5256,7 +6073,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="150372736"/>
+        <c:crossAx val="74970240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5264,7 +6081,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="150372736"/>
+        <c:axId val="74970240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.70000000000000007"/>
@@ -5276,7 +6093,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="150358656"/>
+        <c:crossAx val="74935680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5400,11 +6217,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="150466944"/>
-        <c:axId val="150468480"/>
+        <c:axId val="75039488"/>
+        <c:axId val="75041024"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="150466944"/>
+        <c:axId val="75039488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5413,7 +6230,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="150468480"/>
+        <c:crossAx val="75041024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5421,7 +6238,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="150468480"/>
+        <c:axId val="75041024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.5"/>
@@ -5433,7 +6250,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="150466944"/>
+        <c:crossAx val="75039488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5569,11 +6386,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="150480768"/>
-        <c:axId val="150482304"/>
+        <c:axId val="75057408"/>
+        <c:axId val="75079680"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="150480768"/>
+        <c:axId val="75057408"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -5582,7 +6399,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="150482304"/>
+        <c:crossAx val="75079680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5590,7 +6407,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="150482304"/>
+        <c:axId val="75079680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5601,7 +6418,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="150480768"/>
+        <c:crossAx val="75057408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5927,11 +6744,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="150518400"/>
-        <c:axId val="150806912"/>
+        <c:axId val="74898816"/>
+        <c:axId val="75379840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="150518400"/>
+        <c:axId val="74898816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5941,7 +6758,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="150806912"/>
+        <c:crossAx val="75379840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5950,7 +6767,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="150806912"/>
+        <c:axId val="75379840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5961,7 +6778,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="150518400"/>
+        <c:crossAx val="74898816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6732,6 +7549,454 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing24.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>27752</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>9125</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Grafik 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7515225" y="1000125"/>
+          <a:ext cx="6580952" cy="3200000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing25.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>237474</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>104456</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Grafik 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8496300" y="1552575"/>
+          <a:ext cx="5209524" cy="2552381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>733425</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Diagramm 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing26.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>733425</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Diagramm 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>704850</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>285040</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>37664</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Grafik 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7210425" y="742950"/>
+          <a:ext cx="5676190" cy="3485714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing27.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>733425</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>218252</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>180543</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Grafik 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7086600" y="723900"/>
+          <a:ext cx="6580952" cy="3457143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing28.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>733425</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>323143</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>142481</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Grafik 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7267575" y="990600"/>
+          <a:ext cx="5657143" cy="3152381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing29.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>733425</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>570789</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>56717</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Grafik 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6724650" y="971550"/>
+          <a:ext cx="5685714" cy="3466667"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -44547,8 +45812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P32" sqref="P32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44562,27 +45827,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="31" t="s">
         <v>548</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15" t="s">
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31" t="s">
         <v>519</v>
       </c>
-      <c r="H1" s="15"/>
+      <c r="H1" s="31"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C2" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15" t="s">
+      <c r="C2" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31" t="s">
         <v>86</v>
       </c>
-      <c r="F2" s="15"/>
-      <c r="G2" s="17" t="s">
+      <c r="F2" s="31"/>
+      <c r="G2" s="16" t="s">
         <v>517</v>
       </c>
       <c r="H2" t="s">
@@ -44590,137 +45855,137 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="32" t="s">
         <v>549</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="32" t="s">
         <v>85</v>
       </c>
       <c r="C3">
         <v>17</v>
       </c>
-      <c r="D3" s="21">
+      <c r="D3" s="20">
         <f>C3/G3</f>
         <v>0.27868852459016391</v>
       </c>
       <c r="E3">
         <v>44</v>
       </c>
-      <c r="F3" s="21">
+      <c r="F3" s="20">
         <f>E3/G3</f>
         <v>0.72131147540983609</v>
       </c>
-      <c r="G3" s="24">
+      <c r="G3" s="23">
         <v>61</v>
       </c>
-      <c r="H3" s="21">
+      <c r="H3" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="19">
+      <c r="A4" s="32"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="18">
         <f>C3/C7</f>
         <v>0.56666666666666665</v>
       </c>
-      <c r="D4" s="22">
+      <c r="D4" s="21">
         <f>C3/G7</f>
         <v>8.8541666666666671E-2</v>
       </c>
-      <c r="E4" s="20">
+      <c r="E4" s="19">
         <f>E3/E7</f>
         <v>0.27160493827160492</v>
       </c>
-      <c r="F4" s="22">
+      <c r="F4" s="21">
         <f>E3/G7</f>
         <v>0.22916666666666666</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16" t="s">
+      <c r="A5" s="32"/>
+      <c r="B5" s="32" t="s">
         <v>86</v>
       </c>
       <c r="C5">
         <v>13</v>
       </c>
-      <c r="D5" s="23">
+      <c r="D5" s="22">
         <f>C5/G5</f>
         <v>9.9236641221374045E-2</v>
       </c>
       <c r="E5">
         <v>118</v>
       </c>
-      <c r="F5" s="23">
+      <c r="F5" s="22">
         <f>E5/G5</f>
         <v>0.9007633587786259</v>
       </c>
-      <c r="G5" s="26">
+      <c r="G5" s="25">
         <v>131</v>
       </c>
-      <c r="H5" s="23">
+      <c r="H5" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="19">
+      <c r="A6" s="32"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="18">
         <f>C5/C7</f>
         <v>0.43333333333333335</v>
       </c>
-      <c r="D6" s="22">
+      <c r="D6" s="21">
         <f>C5/G7</f>
         <v>6.7708333333333329E-2</v>
       </c>
-      <c r="E6" s="20">
+      <c r="E6" s="19">
         <f>E5/E7</f>
         <v>0.72839506172839508</v>
       </c>
-      <c r="F6" s="22">
+      <c r="F6" s="21">
         <f>E5/G7</f>
         <v>0.61458333333333337</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="32" t="s">
         <v>519</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="16" t="s">
         <v>517</v>
       </c>
-      <c r="C7" s="28">
+      <c r="C7" s="27">
         <v>30</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="26">
         <v>162</v>
       </c>
-      <c r="G7" s="25">
+      <c r="G7" s="24">
         <f>SUM(G3:G6)</f>
         <v>192</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
+      <c r="A8" s="32"/>
       <c r="B8" t="s">
         <v>518</v>
       </c>
-      <c r="C8" s="19">
-        <v>1</v>
-      </c>
-      <c r="E8" s="20">
-        <v>1</v>
-      </c>
-      <c r="H8" s="30">
+      <c r="C8" s="18">
+        <v>1</v>
+      </c>
+      <c r="E8" s="19">
+        <v>1</v>
+      </c>
+      <c r="H8" s="29">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="31" t="s">
         <v>548</v>
       </c>
-      <c r="D12" s="15"/>
+      <c r="D12" s="31"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
@@ -44734,7 +45999,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="32" t="s">
         <v>549</v>
       </c>
       <c r="B14" t="s">
@@ -44754,7 +46019,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="16"/>
+      <c r="A15" s="32"/>
       <c r="B15" t="s">
         <v>86</v>
       </c>
@@ -44789,14 +46054,14 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="31" t="s">
         <v>548</v>
       </c>
-      <c r="D19" s="15"/>
+      <c r="D19" s="31"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
@@ -44807,53 +46072,53 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="32" t="s">
         <v>549</v>
       </c>
       <c r="B21" t="s">
         <v>534</v>
       </c>
-      <c r="C21" s="31">
+      <c r="C21" s="30">
         <f>C14/C16</f>
         <v>0.56666666666666665</v>
       </c>
-      <c r="D21" s="31">
+      <c r="D21" s="30">
         <f>D14/D16</f>
         <v>0.27160493827160492</v>
       </c>
-      <c r="E21" s="18"/>
+      <c r="E21" s="17"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="16"/>
+      <c r="A22" s="32"/>
       <c r="B22" t="s">
         <v>535</v>
       </c>
-      <c r="C22" s="31">
+      <c r="C22" s="30">
         <f>C15/C16</f>
         <v>0.43333333333333335</v>
       </c>
-      <c r="D22" s="31">
+      <c r="D22" s="30">
         <f>D15/D16</f>
         <v>0.72839506172839508</v>
       </c>
-      <c r="E22" s="18"/>
+      <c r="E22" s="17"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>518</v>
       </c>
-      <c r="C23" s="29">
+      <c r="C23" s="28">
         <f>C21+C22</f>
         <v>1</v>
       </c>
-      <c r="D23" s="29">
+      <c r="D23" s="28">
         <f>D21+D22</f>
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -44894,27 +46159,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="31" t="s">
         <v>548</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15" t="s">
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31" t="s">
         <v>519</v>
       </c>
-      <c r="H1" s="15"/>
+      <c r="H1" s="31"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C2" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15" t="s">
+      <c r="C2" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31" t="s">
         <v>86</v>
       </c>
-      <c r="F2" s="15"/>
-      <c r="G2" s="17" t="s">
+      <c r="F2" s="31"/>
+      <c r="G2" s="16" t="s">
         <v>517</v>
       </c>
       <c r="H2" t="s">
@@ -44922,137 +46187,137 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="32" t="s">
         <v>550</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="32" t="s">
         <v>85</v>
       </c>
       <c r="C3">
         <v>26</v>
       </c>
-      <c r="D3" s="21">
+      <c r="D3" s="20">
         <f>C3/G3</f>
         <v>0.42622950819672129</v>
       </c>
       <c r="E3">
         <v>127</v>
       </c>
-      <c r="F3" s="21">
+      <c r="F3" s="20">
         <f>E3/G3</f>
         <v>2.081967213114754</v>
       </c>
-      <c r="G3" s="24">
+      <c r="G3" s="23">
         <v>61</v>
       </c>
-      <c r="H3" s="21">
+      <c r="H3" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="19">
+      <c r="A4" s="32"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="18">
         <f>C3/C7</f>
         <v>0.8666666666666667</v>
       </c>
-      <c r="D4" s="22">
+      <c r="D4" s="21">
         <f>C3/G7</f>
         <v>0.13541666666666666</v>
       </c>
-      <c r="E4" s="20">
+      <c r="E4" s="19">
         <f>E3/E7</f>
         <v>0.78395061728395066</v>
       </c>
-      <c r="F4" s="22">
+      <c r="F4" s="21">
         <f>E3/G7</f>
         <v>0.66145833333333337</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16" t="s">
+      <c r="A5" s="32"/>
+      <c r="B5" s="32" t="s">
         <v>86</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
-      <c r="D5" s="23">
+      <c r="D5" s="22">
         <f>C5/G5</f>
         <v>3.0534351145038167E-2</v>
       </c>
       <c r="E5">
         <v>35</v>
       </c>
-      <c r="F5" s="23">
+      <c r="F5" s="22">
         <f>E5/G5</f>
         <v>0.26717557251908397</v>
       </c>
-      <c r="G5" s="26">
+      <c r="G5" s="25">
         <v>131</v>
       </c>
-      <c r="H5" s="23">
+      <c r="H5" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="19">
+      <c r="A6" s="32"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="18">
         <f>C5/C7</f>
         <v>0.13333333333333333</v>
       </c>
-      <c r="D6" s="22">
+      <c r="D6" s="21">
         <f>C5/G7</f>
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="E6" s="20">
+      <c r="E6" s="19">
         <f>E5/E7</f>
         <v>0.21604938271604937</v>
       </c>
-      <c r="F6" s="22">
+      <c r="F6" s="21">
         <f>E5/G7</f>
         <v>0.18229166666666666</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="32" t="s">
         <v>519</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="16" t="s">
         <v>517</v>
       </c>
-      <c r="C7" s="28">
+      <c r="C7" s="27">
         <v>30</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="26">
         <v>162</v>
       </c>
-      <c r="G7" s="25">
+      <c r="G7" s="24">
         <f>SUM(G3:G6)</f>
         <v>192</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
+      <c r="A8" s="32"/>
       <c r="B8" t="s">
         <v>518</v>
       </c>
-      <c r="C8" s="19">
-        <v>1</v>
-      </c>
-      <c r="E8" s="20">
-        <v>1</v>
-      </c>
-      <c r="H8" s="30">
+      <c r="C8" s="18">
+        <v>1</v>
+      </c>
+      <c r="E8" s="19">
+        <v>1</v>
+      </c>
+      <c r="H8" s="29">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="31" t="s">
         <v>548</v>
       </c>
-      <c r="D12" s="15"/>
+      <c r="D12" s="31"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
@@ -45066,7 +46331,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="32" t="s">
         <v>550</v>
       </c>
       <c r="B14" t="s">
@@ -45086,7 +46351,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="16"/>
+      <c r="A15" s="32"/>
       <c r="B15" t="s">
         <v>86</v>
       </c>
@@ -45121,14 +46386,14 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="31" t="s">
         <v>548</v>
       </c>
-      <c r="D19" s="15"/>
+      <c r="D19" s="31"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
@@ -45139,61 +46404,56 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="32" t="s">
         <v>550</v>
       </c>
       <c r="B21" t="s">
         <v>534</v>
       </c>
-      <c r="C21" s="31">
+      <c r="C21" s="30">
         <f>C14/C16</f>
         <v>0.8666666666666667</v>
       </c>
-      <c r="D21" s="31">
+      <c r="D21" s="30">
         <f>D14/D16</f>
         <v>0.78395061728395066</v>
       </c>
-      <c r="E21" s="18"/>
+      <c r="E21" s="17"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="16"/>
+      <c r="A22" s="32"/>
       <c r="B22" t="s">
         <v>535</v>
       </c>
-      <c r="C22" s="31">
+      <c r="C22" s="30">
         <f>C15/C16</f>
         <v>0.13333333333333333</v>
       </c>
-      <c r="D22" s="31">
+      <c r="D22" s="30">
         <f>D15/D16</f>
         <v>0.21604938271604937</v>
       </c>
-      <c r="E22" s="18"/>
+      <c r="E22" s="17"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>518</v>
       </c>
-      <c r="C23" s="29">
+      <c r="C23" s="28">
         <f>C21+C22</f>
         <v>1</v>
       </c>
-      <c r="D23" s="29">
+      <c r="D23" s="28">
         <f>D21+D22</f>
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="A21:A22"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="C2:D2"/>
@@ -45201,6 +46461,306 @@
     <mergeCell ref="A3:A6"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="B5:B6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="A21:A22"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" customWidth="1"/>
+    <col min="4" max="4" width="6" customWidth="1"/>
+    <col min="5" max="5" width="7.28515625" customWidth="1"/>
+    <col min="6" max="6" width="6.85546875" customWidth="1"/>
+    <col min="7" max="7" width="6.140625" customWidth="1"/>
+    <col min="8" max="8" width="7" customWidth="1"/>
+    <col min="9" max="9" width="6.140625" customWidth="1"/>
+    <col min="10" max="10" width="6" customWidth="1"/>
+    <col min="11" max="11" width="6.42578125" customWidth="1"/>
+    <col min="12" max="12" width="6.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C1" s="31" t="s">
+        <v>552</v>
+      </c>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31" t="s">
+        <v>519</v>
+      </c>
+      <c r="L1" s="31"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C2" s="31">
+        <v>1</v>
+      </c>
+      <c r="D2" s="31"/>
+      <c r="E2" s="33" t="s">
+        <v>523</v>
+      </c>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33" t="s">
+        <v>524</v>
+      </c>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="J2" s="33"/>
+      <c r="K2" s="16" t="s">
+        <v>517</v>
+      </c>
+      <c r="L2" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="32" t="s">
+        <v>551</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="15">
+        <v>0</v>
+      </c>
+      <c r="D3" s="42">
+        <v>0</v>
+      </c>
+      <c r="E3" s="34">
+        <v>50</v>
+      </c>
+      <c r="F3" s="38">
+        <f>E3/K3</f>
+        <v>0.51546391752577314</v>
+      </c>
+      <c r="G3" s="34">
+        <v>43</v>
+      </c>
+      <c r="H3" s="38">
+        <f>G3/K3</f>
+        <v>0.44329896907216493</v>
+      </c>
+      <c r="I3" s="34">
+        <v>4</v>
+      </c>
+      <c r="J3" s="39">
+        <f>I3/K3</f>
+        <v>4.1237113402061855E-2</v>
+      </c>
+      <c r="K3" s="36">
+        <v>97</v>
+      </c>
+      <c r="L3" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="32"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="34"/>
+      <c r="L4" s="34"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="32" t="s">
+        <v>519</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>517</v>
+      </c>
+      <c r="C5" s="16">
+        <v>0</v>
+      </c>
+      <c r="D5" s="16"/>
+      <c r="E5" s="36">
+        <v>50</v>
+      </c>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34">
+        <v>43</v>
+      </c>
+      <c r="H5" s="34"/>
+      <c r="I5" s="34">
+        <v>4</v>
+      </c>
+      <c r="J5" s="34"/>
+      <c r="K5" s="34">
+        <f>SUM(K3:K4)</f>
+        <v>97</v>
+      </c>
+      <c r="L5" s="34"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="32"/>
+      <c r="B6" t="s">
+        <v>518</v>
+      </c>
+      <c r="C6" s="28">
+        <v>1</v>
+      </c>
+      <c r="E6" s="35">
+        <v>1</v>
+      </c>
+      <c r="F6" s="34"/>
+      <c r="G6" s="35">
+        <v>1</v>
+      </c>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35">
+        <v>1</v>
+      </c>
+      <c r="J6" s="34"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" s="41" t="s">
+        <v>523</v>
+      </c>
+      <c r="F10" s="41" t="s">
+        <v>524</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>517</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>50</v>
+      </c>
+      <c r="F11">
+        <v>43</v>
+      </c>
+      <c r="G11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="40"/>
+      <c r="B12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" t="s">
+        <v>518</v>
+      </c>
+      <c r="D12" s="28">
+        <v>0</v>
+      </c>
+      <c r="E12" s="39">
+        <v>0.51549999999999996</v>
+      </c>
+      <c r="F12" s="39">
+        <v>0.44330000000000003</v>
+      </c>
+      <c r="G12" s="39">
+        <v>4.1200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="40"/>
+      <c r="B13" t="s">
+        <v>519</v>
+      </c>
+      <c r="C13" t="s">
+        <v>518</v>
+      </c>
+      <c r="D13" s="39">
+        <v>0</v>
+      </c>
+      <c r="E13" s="39">
+        <v>0.56770833333333337</v>
+      </c>
+      <c r="F13" s="39">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="G13" s="39">
+        <v>4.6875E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="40"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="40"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="C1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -45367,6 +46927,1155 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="6.42578125" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" customWidth="1"/>
+    <col min="5" max="5" width="7.28515625" customWidth="1"/>
+    <col min="6" max="6" width="6.85546875" customWidth="1"/>
+    <col min="7" max="7" width="6.42578125" customWidth="1"/>
+    <col min="8" max="8" width="6.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C1" s="31" t="s">
+        <v>553</v>
+      </c>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31" t="s">
+        <v>519</v>
+      </c>
+      <c r="H1" s="31"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C2" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="31"/>
+      <c r="E2" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="F2" s="33"/>
+      <c r="G2" s="16" t="s">
+        <v>517</v>
+      </c>
+      <c r="H2" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="32" t="s">
+        <v>551</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="15">
+        <v>84</v>
+      </c>
+      <c r="D3" s="43">
+        <f>C3/G3</f>
+        <v>0.865979381443299</v>
+      </c>
+      <c r="E3" s="34">
+        <v>13</v>
+      </c>
+      <c r="F3" s="38">
+        <f>E3/G3</f>
+        <v>0.13402061855670103</v>
+      </c>
+      <c r="G3" s="36">
+        <v>97</v>
+      </c>
+      <c r="H3" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="32"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="32" t="s">
+        <v>519</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>517</v>
+      </c>
+      <c r="C5" s="16">
+        <v>84</v>
+      </c>
+      <c r="D5" s="16"/>
+      <c r="E5" s="36">
+        <v>13</v>
+      </c>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34">
+        <f>SUM(G3:G4)</f>
+        <v>97</v>
+      </c>
+      <c r="H5" s="34"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="32"/>
+      <c r="B6" t="s">
+        <v>518</v>
+      </c>
+      <c r="C6" s="28">
+        <v>1</v>
+      </c>
+      <c r="E6" s="35">
+        <v>1</v>
+      </c>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>85</v>
+      </c>
+      <c r="E10" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="F10" s="41"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>517</v>
+      </c>
+      <c r="D11">
+        <v>84</v>
+      </c>
+      <c r="E11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="40"/>
+      <c r="B12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" t="s">
+        <v>518</v>
+      </c>
+      <c r="D12" s="39">
+        <f>D3</f>
+        <v>0.865979381443299</v>
+      </c>
+      <c r="E12" s="39">
+        <f>F3</f>
+        <v>0.13402061855670103</v>
+      </c>
+      <c r="F12" s="39"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="40"/>
+      <c r="B13" t="s">
+        <v>519</v>
+      </c>
+      <c r="C13" t="s">
+        <v>518</v>
+      </c>
+      <c r="D13" s="39">
+        <v>0.88</v>
+      </c>
+      <c r="E13" s="39">
+        <v>0.12</v>
+      </c>
+      <c r="F13" s="39"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="40"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="40"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="6.42578125" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" customWidth="1"/>
+    <col min="5" max="5" width="7.28515625" customWidth="1"/>
+    <col min="6" max="6" width="6.85546875" customWidth="1"/>
+    <col min="7" max="7" width="6.42578125" customWidth="1"/>
+    <col min="8" max="8" width="6.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C1" s="31" t="s">
+        <v>548</v>
+      </c>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31" t="s">
+        <v>519</v>
+      </c>
+      <c r="H1" s="31"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C2" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="31"/>
+      <c r="E2" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="F2" s="33"/>
+      <c r="G2" s="16" t="s">
+        <v>517</v>
+      </c>
+      <c r="H2" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="32" t="s">
+        <v>551</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="15">
+        <v>19</v>
+      </c>
+      <c r="D3" s="43">
+        <f>C3/G3</f>
+        <v>0.19587628865979381</v>
+      </c>
+      <c r="E3" s="34">
+        <v>78</v>
+      </c>
+      <c r="F3" s="38">
+        <f>E3/G3</f>
+        <v>0.80412371134020622</v>
+      </c>
+      <c r="G3" s="36">
+        <v>97</v>
+      </c>
+      <c r="H3" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="32"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="32" t="s">
+        <v>519</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>517</v>
+      </c>
+      <c r="C5" s="16">
+        <f>C3</f>
+        <v>19</v>
+      </c>
+      <c r="D5" s="16"/>
+      <c r="E5" s="36">
+        <f>E3</f>
+        <v>78</v>
+      </c>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34">
+        <f>SUM(G3:G4)</f>
+        <v>97</v>
+      </c>
+      <c r="H5" s="34"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="32"/>
+      <c r="B6" t="s">
+        <v>518</v>
+      </c>
+      <c r="C6" s="28">
+        <v>1</v>
+      </c>
+      <c r="E6" s="35">
+        <v>1</v>
+      </c>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>85</v>
+      </c>
+      <c r="E10" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="F10" s="41"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>517</v>
+      </c>
+      <c r="D11">
+        <v>84</v>
+      </c>
+      <c r="E11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="40"/>
+      <c r="B12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" t="s">
+        <v>518</v>
+      </c>
+      <c r="D12" s="39">
+        <f>D3</f>
+        <v>0.19587628865979381</v>
+      </c>
+      <c r="E12" s="39">
+        <f>F3</f>
+        <v>0.80412371134020622</v>
+      </c>
+      <c r="F12" s="39"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="40"/>
+      <c r="B13" t="s">
+        <v>519</v>
+      </c>
+      <c r="C13" t="s">
+        <v>518</v>
+      </c>
+      <c r="D13" s="39">
+        <v>0.156</v>
+      </c>
+      <c r="E13" s="39">
+        <v>0.84399999999999997</v>
+      </c>
+      <c r="F13" s="39"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F14" s="39">
+        <f>D12-D13</f>
+        <v>3.9876288659793813E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="40"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="40"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="6" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" customWidth="1"/>
+    <col min="6" max="6" width="6.85546875" customWidth="1"/>
+    <col min="7" max="7" width="7.28515625" customWidth="1"/>
+    <col min="8" max="8" width="6.85546875" customWidth="1"/>
+    <col min="9" max="9" width="6.42578125" customWidth="1"/>
+    <col min="10" max="10" width="6.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E1" s="16" t="s">
+        <v>554</v>
+      </c>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="31" t="s">
+        <v>519</v>
+      </c>
+      <c r="J1" s="31"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C2" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="F2" s="31"/>
+      <c r="G2" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="H2" s="33"/>
+      <c r="I2" s="16" t="s">
+        <v>517</v>
+      </c>
+      <c r="J2" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="32" t="s">
+        <v>551</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="15">
+        <v>64</v>
+      </c>
+      <c r="D3" s="43">
+        <f>C3/I3</f>
+        <v>0.65979381443298968</v>
+      </c>
+      <c r="E3" s="15">
+        <v>26</v>
+      </c>
+      <c r="F3" s="43">
+        <f>E3/I3</f>
+        <v>0.26804123711340205</v>
+      </c>
+      <c r="G3" s="34">
+        <v>7</v>
+      </c>
+      <c r="H3" s="38">
+        <f>G3/I3</f>
+        <v>7.2164948453608241E-2</v>
+      </c>
+      <c r="I3" s="36">
+        <v>97</v>
+      </c>
+      <c r="J3" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="32"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="32" t="s">
+        <v>519</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>517</v>
+      </c>
+      <c r="C5" s="16">
+        <f>C3</f>
+        <v>64</v>
+      </c>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16">
+        <f>E3</f>
+        <v>26</v>
+      </c>
+      <c r="F5" s="16"/>
+      <c r="G5" s="36">
+        <f>G3</f>
+        <v>7</v>
+      </c>
+      <c r="H5" s="34"/>
+      <c r="I5" s="34">
+        <f>SUM(I3:I4)</f>
+        <v>97</v>
+      </c>
+      <c r="J5" s="34"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="32"/>
+      <c r="B6" t="s">
+        <v>518</v>
+      </c>
+      <c r="C6" s="28">
+        <v>1</v>
+      </c>
+      <c r="E6" s="28">
+        <v>1</v>
+      </c>
+      <c r="G6" s="35">
+        <v>1</v>
+      </c>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="D10" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="E10" t="s">
+        <v>85</v>
+      </c>
+      <c r="F10" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="G10" s="41"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>517</v>
+      </c>
+      <c r="E11">
+        <v>84</v>
+      </c>
+      <c r="F11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="40"/>
+      <c r="B12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" t="s">
+        <v>518</v>
+      </c>
+      <c r="D12" s="39">
+        <f>D3</f>
+        <v>0.65979381443298968</v>
+      </c>
+      <c r="E12" s="39">
+        <f>F3</f>
+        <v>0.26804123711340205</v>
+      </c>
+      <c r="F12" s="39">
+        <f>H3</f>
+        <v>7.2164948453608241E-2</v>
+      </c>
+      <c r="G12" s="39"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="40"/>
+      <c r="B13" t="s">
+        <v>519</v>
+      </c>
+      <c r="C13" t="s">
+        <v>518</v>
+      </c>
+      <c r="D13" s="28">
+        <v>0.63</v>
+      </c>
+      <c r="E13" s="39">
+        <v>0.26</v>
+      </c>
+      <c r="F13" s="39">
+        <v>0.109</v>
+      </c>
+      <c r="G13" s="39"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G14" s="39"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="40"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="30"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="40"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="30"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="6.42578125" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" customWidth="1"/>
+    <col min="5" max="5" width="7.28515625" customWidth="1"/>
+    <col min="6" max="6" width="6.85546875" customWidth="1"/>
+    <col min="7" max="7" width="6.42578125" customWidth="1"/>
+    <col min="8" max="8" width="6.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C1" s="31" t="s">
+        <v>550</v>
+      </c>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31" t="s">
+        <v>519</v>
+      </c>
+      <c r="H1" s="31"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C2" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="31"/>
+      <c r="E2" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="F2" s="33"/>
+      <c r="G2" s="16" t="s">
+        <v>517</v>
+      </c>
+      <c r="H2" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="32" t="s">
+        <v>551</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="15">
+        <v>86</v>
+      </c>
+      <c r="D3" s="43">
+        <f>C3/G3</f>
+        <v>0.88659793814432986</v>
+      </c>
+      <c r="E3" s="34">
+        <v>11</v>
+      </c>
+      <c r="F3" s="38">
+        <f>E3/G3</f>
+        <v>0.1134020618556701</v>
+      </c>
+      <c r="G3" s="36">
+        <v>97</v>
+      </c>
+      <c r="H3" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="32"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="32" t="s">
+        <v>519</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>517</v>
+      </c>
+      <c r="C5" s="16">
+        <f>C3</f>
+        <v>86</v>
+      </c>
+      <c r="D5" s="16"/>
+      <c r="E5" s="36">
+        <f>E3</f>
+        <v>11</v>
+      </c>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34">
+        <f>SUM(G3:G4)</f>
+        <v>97</v>
+      </c>
+      <c r="H5" s="34"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="32"/>
+      <c r="B6" t="s">
+        <v>518</v>
+      </c>
+      <c r="C6" s="28">
+        <v>1</v>
+      </c>
+      <c r="E6" s="35">
+        <v>1</v>
+      </c>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>85</v>
+      </c>
+      <c r="E10" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="F10" s="41"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>517</v>
+      </c>
+      <c r="D11">
+        <v>84</v>
+      </c>
+      <c r="E11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="40"/>
+      <c r="B12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" t="s">
+        <v>518</v>
+      </c>
+      <c r="D12" s="39">
+        <f>D3</f>
+        <v>0.88659793814432986</v>
+      </c>
+      <c r="E12" s="39">
+        <f>F3</f>
+        <v>0.1134020618556701</v>
+      </c>
+      <c r="F12" s="39"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="40"/>
+      <c r="B13" t="s">
+        <v>519</v>
+      </c>
+      <c r="C13" t="s">
+        <v>518</v>
+      </c>
+      <c r="D13" s="39">
+        <v>0.79700000000000004</v>
+      </c>
+      <c r="E13" s="39">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="F13" s="39"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F14" s="39">
+        <f>D12-D13</f>
+        <v>8.9597938144329814E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="40"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="40"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="6.42578125" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" customWidth="1"/>
+    <col min="5" max="5" width="7.28515625" customWidth="1"/>
+    <col min="6" max="6" width="6.85546875" customWidth="1"/>
+    <col min="7" max="7" width="6.42578125" customWidth="1"/>
+    <col min="8" max="8" width="6.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C1" s="31" t="s">
+        <v>549</v>
+      </c>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31" t="s">
+        <v>519</v>
+      </c>
+      <c r="H1" s="31"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C2" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="31"/>
+      <c r="E2" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="F2" s="33"/>
+      <c r="G2" s="16" t="s">
+        <v>517</v>
+      </c>
+      <c r="H2" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="32" t="s">
+        <v>551</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="15">
+        <v>34</v>
+      </c>
+      <c r="D3" s="43">
+        <f>C3/G3</f>
+        <v>0.35051546391752575</v>
+      </c>
+      <c r="E3" s="34">
+        <v>63</v>
+      </c>
+      <c r="F3" s="38">
+        <f>E3/G3</f>
+        <v>0.64948453608247425</v>
+      </c>
+      <c r="G3" s="36">
+        <v>97</v>
+      </c>
+      <c r="H3" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="32"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="32" t="s">
+        <v>519</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>517</v>
+      </c>
+      <c r="C5" s="16">
+        <f>C3</f>
+        <v>34</v>
+      </c>
+      <c r="D5" s="16"/>
+      <c r="E5" s="36">
+        <f>E3</f>
+        <v>63</v>
+      </c>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34">
+        <f>SUM(G3:G4)</f>
+        <v>97</v>
+      </c>
+      <c r="H5" s="34"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="32"/>
+      <c r="B6" t="s">
+        <v>518</v>
+      </c>
+      <c r="C6" s="28">
+        <v>1</v>
+      </c>
+      <c r="E6" s="35">
+        <v>1</v>
+      </c>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>85</v>
+      </c>
+      <c r="E10" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="F10" s="41"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>517</v>
+      </c>
+      <c r="D11">
+        <v>84</v>
+      </c>
+      <c r="E11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="40"/>
+      <c r="B12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" t="s">
+        <v>518</v>
+      </c>
+      <c r="D12" s="39">
+        <f>D3</f>
+        <v>0.35051546391752575</v>
+      </c>
+      <c r="E12" s="39">
+        <f>F3</f>
+        <v>0.64948453608247425</v>
+      </c>
+      <c r="F12" s="39"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="40"/>
+      <c r="B13" t="s">
+        <v>519</v>
+      </c>
+      <c r="C13" t="s">
+        <v>518</v>
+      </c>
+      <c r="D13" s="39">
+        <v>0.318</v>
+      </c>
+      <c r="E13" s="39">
+        <v>0.68200000000000005</v>
+      </c>
+      <c r="F13" s="39"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F14" s="39"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="40"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="40"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I6"/>
@@ -45518,7 +48227,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="B3" sqref="B3:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>